<commit_message>
Add implementations for FirstOccurrence, InsertionSort, and TwoSum classes
</commit_message>
<xml_diff>
--- a/Factorial and Fibonacci.xlsx
+++ b/Factorial and Fibonacci.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debdootmanna/VSCode/DAA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13E0615E-1EDC-2C40-9BEC-34F54A191D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C6068C-BA32-184C-B527-ED71F81E933C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="2060" windowWidth="28040" windowHeight="17440" xr2:uid="{61D9F596-1B55-1043-8530-72E348AA0CF6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="21380" xr2:uid="{61D9F596-1B55-1043-8530-72E348AA0CF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
   <si>
     <t>N</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>O(n)</t>
+  </si>
+  <si>
+    <t>y = 3x + 2</t>
   </si>
 </sst>
 </file>
@@ -88,10 +91,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -145,7 +154,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Fibonacci Series</a:t>
+              <a:t>Fibonacci Itteration Series</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -580,7 +589,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Factorial Series</a:t>
+              <a:t>Factorial Itteration Series</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -980,6 +989,423 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Fibonacci</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Recursive Series</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$52:$A$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$52:$B$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-025C-884F-8463-CE7A685E0B51}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1747471056"/>
+        <c:axId val="1747525760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1747471056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1747525760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1747525760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1747471056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1060,6 +1486,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1577,6 +2043,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2097,15 +3079,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:colOff>6687</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>6294</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>651858</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>56195</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2133,15 +3115,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>10565</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>451</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>450850</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>134868</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>67434</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2163,6 +3145,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>815948</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>5169</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>465293</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>118457</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54D11F79-F6E4-3BB3-1D67-E8E851CBF027}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2468,10 +3486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4548C506-C800-FA4E-BE69-FA088C7A4ED1}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="113" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2692,12 +3710,80 @@
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
     </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>17</v>
+      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>10</v>
+      </c>
+      <c r="B54">
+        <v>32</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>15</v>
+      </c>
+      <c r="B55">
+        <v>47</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>20</v>
+      </c>
+      <c r="B56">
+        <v>62</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="C2:C10"/>
     <mergeCell ref="D2:D10"/>
     <mergeCell ref="C27:C35"/>
     <mergeCell ref="D27:D35"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="D52:D56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>